<commit_message>
modif url VS (#57) c6c8ff5c025969e5a09e6e105911c4f8977d57a4
</commit_message>
<xml_diff>
--- a/ig/main/eclaire-study-status-concept-map.xlsx
+++ b/ig/main/eclaire-study-status-concept-map.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-01T14:26:19+00:00</t>
+    <t>2023-09-01T14:41:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -96,7 +96,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/R4/valueset-research-study-status</t>
+    <t>http://hl7.org/fhir/ValueSet/research-study-status</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>